<commit_message>
Changes to data summary.
</commit_message>
<xml_diff>
--- a/DataSummary.xlsx
+++ b/DataSummary.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw/Desktop/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw/git/SDC_Term1_P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E3DBCF87-7C35-4C47-BA29-70F6050C2898}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{373C172D-6FD9-4641-AB6F-9D8AE3D3D917}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{44F190E4-B0DA-4F46-9E6C-4FC298ACD4F9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{44F190E4-B0DA-4F46-9E6C-4FC298ACD4F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Models" sheetId="2" r:id="rId2"/>
+    <sheet name="Network" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Dataset</t>
   </si>
@@ -48,10 +50,160 @@
     <t xml:space="preserve">Size </t>
   </si>
   <si>
-    <t>Centering from edges</t>
-  </si>
-  <si>
     <t>General driving, center of lane</t>
+  </si>
+  <si>
+    <t>Train3</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Centering from edges, starting parallel to edges</t>
+  </si>
+  <si>
+    <t>Centering from edges, starting pointed at edges; over bridge</t>
+  </si>
+  <si>
+    <t>Not sure if this data collection was the best… started recording too early sometimes.</t>
+  </si>
+  <si>
+    <t>Model Name</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>LeNet1</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>LeNet</t>
+  </si>
+  <si>
+    <t>MaxPool - f2 s2</t>
+  </si>
+  <si>
+    <t>conv d20 f5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer </t>
+  </si>
+  <si>
+    <t>Flatten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dense 120 </t>
+  </si>
+  <si>
+    <t>Dense 84</t>
+  </si>
+  <si>
+    <t>Dense 1</t>
+  </si>
+  <si>
+    <t>Training Set</t>
+  </si>
+  <si>
+    <t>model_2</t>
+  </si>
+  <si>
+    <t>model_1</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>1,2,</t>
+  </si>
+  <si>
+    <t>Off road before bridge</t>
+  </si>
+  <si>
+    <t>Off road before bridge - sharper angles towards edges - Train3 probably not so good</t>
+  </si>
+  <si>
+    <t>nvidia</t>
+  </si>
+  <si>
+    <t>model_3</t>
+  </si>
+  <si>
+    <t>Track 1</t>
+  </si>
+  <si>
+    <t>Track 2</t>
+  </si>
+  <si>
+    <t>Ran into wall on bridge</t>
+  </si>
+  <si>
+    <t>Major fail</t>
+  </si>
+  <si>
+    <t>Conv - d24 f5 s2</t>
+  </si>
+  <si>
+    <t>Conv - d10 f5 s1</t>
+  </si>
+  <si>
+    <t>Conv - d36 f5 s2</t>
+  </si>
+  <si>
+    <t>Conv - d48 f5 s2</t>
+  </si>
+  <si>
+    <t>Conv - d64 f5 s1</t>
+  </si>
+  <si>
+    <t>Dense 1000</t>
+  </si>
+  <si>
+    <t>Dense 100</t>
+  </si>
+  <si>
+    <t>Dense 50</t>
+  </si>
+  <si>
+    <t>conv d20 f5 s1</t>
+  </si>
+  <si>
+    <t>Train4</t>
+  </si>
+  <si>
+    <t>Center of lane</t>
+  </si>
+  <si>
+    <t>Train5</t>
+  </si>
+  <si>
+    <t>Across bridge forward and backwards, some of the track backwards</t>
+  </si>
+  <si>
+    <t>model_4</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Steering correction wrong</t>
+  </si>
+  <si>
+    <t>Corrected steering issue</t>
+  </si>
+  <si>
+    <t>model_5</t>
+  </si>
+  <si>
+    <t>1,2,4,5</t>
   </si>
 </sst>
 </file>
@@ -67,12 +219,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,9 +245,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165F296F-CC9F-FA42-B17F-FC1D6F9CE351}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -418,7 +587,7 @@
     <col min="5" max="5" width="56.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +603,11 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -449,10 +621,10 @@
         <v>1505</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -466,7 +638,494 @@
         <v>462</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43284</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>763</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43284</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1249</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43284</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>853</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E06421F-EE9B-1345-8678-6856D934A741}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="39.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="44.5" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C256F8-A55E-3143-8719-D96CED60F423}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved work into a python notebook, so model.py is slightly out of date. Working on data analysis, etc.
</commit_message>
<xml_diff>
--- a/DataSummary.xlsx
+++ b/DataSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw/git/SDC_Term1_P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{373C172D-6FD9-4641-AB6F-9D8AE3D3D917}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4D3C4979-4D33-C346-A4C4-9440368E0FF3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{44F190E4-B0DA-4F46-9E6C-4FC298ACD4F9}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
   <si>
     <t>Dataset</t>
   </si>
@@ -204,6 +204,60 @@
   </si>
   <si>
     <t>1,2,4,5</t>
+  </si>
+  <si>
+    <t>Wrong dropout rate</t>
+  </si>
+  <si>
+    <t>model_6</t>
+  </si>
+  <si>
+    <t>Oscillates left and right, along sides of road</t>
+  </si>
+  <si>
+    <t>Fixed dropout issue from model_5. Steering correction et at +/- 1.5 -&gt; may be too high.</t>
+  </si>
+  <si>
+    <t>model_7</t>
+  </si>
+  <si>
+    <t>Better but still oscillating</t>
+  </si>
+  <si>
+    <t>model_8</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>model_9</t>
+  </si>
+  <si>
+    <t>Did fairly well; off the road after the bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See shadow and immediately veers off the road; need something to correct for this. </t>
+  </si>
+  <si>
+    <t>Data Filtering</t>
+  </si>
+  <si>
+    <t>Removed [-0.05, 0.05]</t>
+  </si>
+  <si>
+    <t>Dropout</t>
+  </si>
+  <si>
+    <t>[0, 0.2, 0.2, 0.5]</t>
+  </si>
+  <si>
+    <t>model_10</t>
+  </si>
+  <si>
+    <t>[0, 0.3, 0.3, 0.5]</t>
+  </si>
+  <si>
+    <t>removed 50% of [-0.05, 0.05]</t>
   </si>
 </sst>
 </file>
@@ -219,18 +273,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -245,14 +293,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -573,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165F296F-CC9F-FA42-B17F-FC1D6F9CE351}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,7 +631,7 @@
     <col min="5" max="5" width="56.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -624,7 +668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -641,7 +685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -661,7 +705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -678,7 +722,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -693,6 +737,39 @@
       </c>
       <c r="E6" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>66</v>
+      </c>
+      <c r="I15">
+        <v>200</v>
+      </c>
+      <c r="J15">
+        <f>I15/H15</f>
+        <v>3.0303030303030303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>160</v>
+      </c>
+      <c r="I16">
+        <v>320</v>
+      </c>
+      <c r="J16">
+        <f>I16/H16</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <f>I17/J15</f>
+        <v>79.2</v>
+      </c>
+      <c r="I17">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -702,41 +779,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E06421F-EE9B-1345-8678-6856D934A741}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="39.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="44.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="38.5" customWidth="1"/>
+    <col min="6" max="6" width="39.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="44.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -746,15 +833,18 @@
       <c r="C2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -764,15 +854,18 @@
       <c r="C3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -782,128 +875,230 @@
       <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="5" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates to data summary.
</commit_message>
<xml_diff>
--- a/DataSummary.xlsx
+++ b/DataSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw/git/SDC_Term1_P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4D3C4979-4D33-C346-A4C4-9440368E0FF3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{535DC1F2-1E30-0A4B-B51E-55340549FE99}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{44F190E4-B0DA-4F46-9E6C-4FC298ACD4F9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{44F190E4-B0DA-4F46-9E6C-4FC298ACD4F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
   <si>
     <t>Dataset</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>removed 50% of [-0.05, 0.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constant swerving back and forth… </t>
   </si>
 </sst>
 </file>
@@ -782,7 +785,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1024,7 +1027,9 @@
       <c r="E11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>

</xml_diff>

<commit_message>
Updates for new data and models trained.
</commit_message>
<xml_diff>
--- a/DataSummary.xlsx
+++ b/DataSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw/git/SDC_Term1_P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{93F90906-3082-6348-AE21-0B0454D88CE2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{05051A5F-E3CD-9549-B3DC-F604563E4E37}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{44F190E4-B0DA-4F46-9E6C-4FC298ACD4F9}"/>
+    <workbookView xWindow="680" yWindow="440" windowWidth="24920" windowHeight="15560" activeTab="1" xr2:uid="{44F190E4-B0DA-4F46-9E6C-4FC298ACD4F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="105">
   <si>
     <t>Dataset</t>
   </si>
@@ -267,16 +267,98 @@
   </si>
   <si>
     <t xml:space="preserve">Turns only </t>
+  </si>
+  <si>
+    <t>model_11</t>
+  </si>
+  <si>
+    <t>2, 4, 6</t>
+  </si>
+  <si>
+    <t>Kept 1/3 of [+/- 0.04]</t>
+  </si>
+  <si>
+    <t>[0, 0.0, 0.3, 0.5]</t>
+  </si>
+  <si>
+    <t>Swerving and stays close to line; went off track at water</t>
+  </si>
+  <si>
+    <t>Tried with less dropout; doesn't seem good</t>
+  </si>
+  <si>
+    <t>nvidia1</t>
+  </si>
+  <si>
+    <t>Cropping</t>
+  </si>
+  <si>
+    <t>[74, 20] [60, 60]</t>
+  </si>
+  <si>
+    <t>[50, 20] [0, 0]</t>
+  </si>
+  <si>
+    <t>Doing better; off track after bridge</t>
+  </si>
+  <si>
+    <t>Cropping made a big difference</t>
+  </si>
+  <si>
+    <t>1, 4, 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steering angle correction was totally wrong. Fixed it. </t>
+  </si>
+  <si>
+    <t>Steering Correction</t>
+  </si>
+  <si>
+    <t>Visualized data and found out that this training set was screwing stuff up; too many cases where vehicle was along the line with wheels pointed straight</t>
+  </si>
+  <si>
+    <t>Train7</t>
+  </si>
+  <si>
+    <t>1, 4, 6, 7</t>
+  </si>
+  <si>
+    <t>Doing better, but doesn't correct properly</t>
+  </si>
+  <si>
+    <t>Navigated the track!!!  Does really well on staight parts, sucks on the bridge. Struggles with shadows. Gets stuck if straddling line; need better data of this.</t>
+  </si>
+  <si>
+    <t>ALMOST! Went off the road at one point, and then got stuck on the crazy bridge with the signs on the side. Need more data.</t>
+  </si>
+  <si>
+    <t>nvidia2</t>
+  </si>
+  <si>
+    <t>Kept all</t>
+  </si>
+  <si>
+    <t>Navigated the track, but seemed to do worse</t>
+  </si>
+  <si>
+    <t>Sucked.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -312,6 +394,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165F296F-CC9F-FA42-B17F-FC1D6F9CE351}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,20 +762,23 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>43284</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>462</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -763,6 +850,17 @@
       </c>
       <c r="E7" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43293</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -800,29 +898,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E06421F-EE9B-1345-8678-6856D934A741}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="38.5" customWidth="1"/>
-    <col min="6" max="6" width="39.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="44.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="45.83203125" customWidth="1"/>
+    <col min="5" max="6" width="38.5" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="39.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="44.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -833,23 +932,29 @@
         <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -861,16 +966,20 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -882,16 +991,20 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -903,18 +1016,22 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>52</v>
       </c>
@@ -926,14 +1043,18 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
@@ -945,14 +1066,18 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>60</v>
       </c>
@@ -964,16 +1089,20 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="4"/>
+      <c r="J7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>63</v>
       </c>
@@ -985,14 +1114,18 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8" s="4"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>65</v>
       </c>
@@ -1004,12 +1137,16 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="F9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>67</v>
       </c>
@@ -1019,22 +1156,26 @@
       <c r="C10" s="3">
         <v>4</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
@@ -1044,89 +1185,207 @@
       <c r="C11" s="3">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>75</v>
-      </c>
+      <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes to drive.py to convert to YUV.
</commit_message>
<xml_diff>
--- a/DataSummary.xlsx
+++ b/DataSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw/git/SDC_Term1_P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BDA77EAE-714C-4C42-A731-A58BFE1D6A2F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FDC5D52C-B54E-4440-BE66-6E692E7E3C59}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="440" windowWidth="24920" windowHeight="15560" activeTab="1" xr2:uid="{44F190E4-B0DA-4F46-9E6C-4FC298ACD4F9}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="162">
   <si>
     <t>Dataset</t>
   </si>
@@ -492,6 +492,27 @@
   </si>
   <si>
     <t xml:space="preserve">Confused in the shadows… </t>
+  </si>
+  <si>
+    <t>Stayed along sideline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confused right off the bat… </t>
+  </si>
+  <si>
+    <t>More testing of steering angle correction - 0.23 doesn’t seem good..</t>
+  </si>
+  <si>
+    <t>Off road at shadow before bridge</t>
+  </si>
+  <si>
+    <t>Off road right away</t>
+  </si>
+  <si>
+    <t>Center only</t>
+  </si>
+  <si>
+    <t>Off road at shadow after brdige. Straddled some lines.</t>
   </si>
 </sst>
 </file>
@@ -1169,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E06421F-EE9B-1345-8678-6856D934A741}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2176,7 +2197,7 @@
     </row>
     <row r="31" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>85</v>
@@ -2210,6 +2231,111 @@
       </c>
       <c r="L31" s="3" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="7">
+        <v>0.23</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I32" s="3">
+        <v>3</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0.27</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I33" s="3">
+        <v>3</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I34" s="7">
+        <v>5</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to drive.py to convert to YUV. Upped speed to 10.
</commit_message>
<xml_diff>
--- a/DataSummary.xlsx
+++ b/DataSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw/git/SDC_Term1_P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FDC5D52C-B54E-4440-BE66-6E692E7E3C59}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ABE09034-1475-F544-BEB1-7E8349346147}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="440" windowWidth="24920" windowHeight="15560" activeTab="1" xr2:uid="{44F190E4-B0DA-4F46-9E6C-4FC298ACD4F9}"/>
+    <workbookView xWindow="780" yWindow="440" windowWidth="24820" windowHeight="15560" activeTab="1" xr2:uid="{44F190E4-B0DA-4F46-9E6C-4FC298ACD4F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="165">
   <si>
     <t>Dataset</t>
   </si>
@@ -513,6 +513,15 @@
   </si>
   <si>
     <t>Off road at shadow after brdige. Straddled some lines.</t>
+  </si>
+  <si>
+    <t>FIXED ISSUE WITH DRIVE.PY FILE</t>
+  </si>
+  <si>
+    <t>Navigated. Little shaky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigated. Perfect. Can't go faster than 9. </t>
   </si>
 </sst>
 </file>
@@ -535,7 +544,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +554,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -574,6 +589,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E06421F-EE9B-1345-8678-6856D934A741}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2336,6 +2352,65 @@
       </c>
       <c r="J34" s="2" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>34</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I37" s="7">
+        <v>3</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>